<commit_message>
TPB に wait 追加
</commit_message>
<xml_diff>
--- a/reports/kakukin/score_sheet_example.xlsx
+++ b/reports/kakukin/score_sheet_example.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muzud\OneDrive\ドキュメント\GitHub\sente-win-rate-70-percent-problem\reports\kakukin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3DFD3E5-62FE-432C-BB51-051851FEA98F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{964C9965-14EF-41B1-8AF7-23F13D7C56D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="410" yWindow="650" windowWidth="15250" windowHeight="15670" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="410" yWindow="650" windowWidth="18210" windowHeight="16230" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="CsvDesign" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="33">
   <si>
     <t>A(表)1</t>
     <rPh sb="2" eb="3">
@@ -108,6 +110,96 @@
       <t>ウラ</t>
     </rPh>
     <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>失敗</t>
+  </si>
+  <si>
+    <t>失敗</t>
+    <rPh sb="0" eb="2">
+      <t>シッパイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Aさん(表)1</t>
+  </si>
+  <si>
+    <t>Aさん(表)1</t>
+    <rPh sb="4" eb="5">
+      <t>オモテ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Bさん(表)1</t>
+  </si>
+  <si>
+    <t>Bさん(表)1</t>
+    <rPh sb="4" eb="5">
+      <t>オモテ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Aさん(裏)3</t>
+  </si>
+  <si>
+    <t>Aさん(裏)3</t>
+    <rPh sb="4" eb="5">
+      <t>ウラ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Bさん(裏)2</t>
+  </si>
+  <si>
+    <t>Bさん(裏)2</t>
+    <rPh sb="4" eb="5">
+      <t>ウラ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Aさん(裏)2</t>
+  </si>
+  <si>
+    <t>Aさん(裏)2</t>
+    <rPh sb="4" eb="5">
+      <t>ウラ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>result</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>e1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>n1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>e2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>n2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>no</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>達成でＡさんの勝ち</t>
+  </si>
+  <si>
+    <t>３局目に続く</t>
   </si>
 </sst>
 </file>
@@ -144,7 +236,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -220,11 +312,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -238,17 +354,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -533,7 +665,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
@@ -594,7 +726,7 @@
       <c r="B11" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="11">
+      <c r="D11" s="8">
         <f>SUMIF(F$4:F$8,B11,D$4:D$8)</f>
         <v>0.36</v>
       </c>
@@ -603,13 +735,13 @@
       <c r="B12" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="10">
+      <c r="D12" s="9">
         <f>SUMIF(F$4:F$8,B12,D$4:D$8)</f>
         <v>0.64</v>
       </c>
     </row>
     <row r="13" spans="2:6">
-      <c r="D13" s="11">
+      <c r="D13" s="8">
         <f>SUM(D11:D12)</f>
         <v>1</v>
       </c>
@@ -733,12 +865,10 @@
     </row>
     <row r="13" spans="2:8" ht="18.5" thickBot="1">
       <c r="C13" s="7"/>
-      <c r="D13" s="8"/>
       <c r="E13" s="2"/>
     </row>
     <row r="14" spans="2:8" ht="18.5" thickBot="1">
       <c r="C14" s="7"/>
-      <c r="D14" s="8"/>
       <c r="E14" s="6" t="s">
         <v>12</v>
       </c>
@@ -751,12 +881,10 @@
     </row>
     <row r="15" spans="2:8" ht="18.5" thickBot="1">
       <c r="C15" s="7"/>
-      <c r="D15" s="8"/>
       <c r="E15" s="4"/>
     </row>
     <row r="16" spans="2:8" ht="18.5" thickBot="1">
       <c r="C16" s="7"/>
-      <c r="D16" s="8"/>
       <c r="E16" s="6" t="s">
         <v>3</v>
       </c>
@@ -771,7 +899,7 @@
       <c r="B19" t="s">
         <v>11</v>
       </c>
-      <c r="D19" s="9">
+      <c r="D19" s="8">
         <f>SUMIF(H$4:H$16,B19,F$4:F$16)</f>
         <v>0.23039999999999999</v>
       </c>
@@ -780,7 +908,7 @@
       <c r="B20" t="s">
         <v>6</v>
       </c>
-      <c r="D20" s="9">
+      <c r="D20" s="8">
         <f>SUMIF(H$4:H$16,B20,F$4:F$16)</f>
         <v>0.36</v>
       </c>
@@ -789,13 +917,13 @@
       <c r="B21" t="s">
         <v>10</v>
       </c>
-      <c r="D21" s="10">
+      <c r="D21" s="9">
         <f>SUMIF(H$4:H$16,B21,F$4:F$16)</f>
         <v>0.40960000000000002</v>
       </c>
     </row>
     <row r="22" spans="2:4">
-      <c r="D22" s="9">
+      <c r="D22" s="8">
         <f>SUM(D19:D21)</f>
         <v>1</v>
       </c>
@@ -804,4 +932,403 @@
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5454F7BB-39E8-49E9-8BB9-12FEE61018B7}">
+  <dimension ref="B2:J28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:L30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18"/>
+  <cols>
+    <col min="1" max="2" width="8.58203125" customWidth="1"/>
+    <col min="3" max="3" width="2.58203125" customWidth="1"/>
+    <col min="4" max="4" width="12.58203125" customWidth="1"/>
+    <col min="5" max="5" width="8.58203125" customWidth="1"/>
+    <col min="6" max="6" width="2.58203125" customWidth="1"/>
+    <col min="7" max="7" width="12.58203125" customWidth="1"/>
+    <col min="8" max="8" width="8.58203125" customWidth="1"/>
+    <col min="10" max="10" width="20.58203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:10">
+      <c r="E2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" ht="18.5" thickBot="1"/>
+    <row r="4" spans="2:10" ht="18.5" thickBot="1">
+      <c r="B4" s="14">
+        <v>1</v>
+      </c>
+      <c r="C4" s="13"/>
+      <c r="D4" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="14">
+        <v>0.54</v>
+      </c>
+      <c r="F4" s="19"/>
+      <c r="G4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="14">
+        <v>0.29160000000000003</v>
+      </c>
+      <c r="J4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" ht="10.5" customHeight="1" thickBot="1">
+      <c r="B5" s="11"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="11"/>
+    </row>
+    <row r="6" spans="2:10" ht="10.5" customHeight="1" thickBot="1">
+      <c r="D6" s="4"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="4"/>
+    </row>
+    <row r="7" spans="2:10" ht="18.5" thickBot="1">
+      <c r="D7" s="4"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" s="14">
+        <v>0.19439999999999999</v>
+      </c>
+      <c r="J7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" ht="7.5" customHeight="1" thickBot="1">
+      <c r="D8" s="4"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="11"/>
+    </row>
+    <row r="9" spans="2:10" ht="11" customHeight="1" thickBot="1">
+      <c r="D9" s="4"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="4"/>
+    </row>
+    <row r="10" spans="2:10" ht="18.5" thickBot="1">
+      <c r="D10" s="4"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" s="14">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="J10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" ht="8.5" customHeight="1" thickBot="1">
+      <c r="D11" s="4"/>
+      <c r="F11" s="18"/>
+      <c r="H11" s="11"/>
+    </row>
+    <row r="12" spans="2:10" ht="10" customHeight="1" thickBot="1">
+      <c r="D12" s="4"/>
+      <c r="F12" s="18"/>
+    </row>
+    <row r="13" spans="2:10" ht="18.5" thickBot="1">
+      <c r="D13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="14">
+        <v>0.36</v>
+      </c>
+      <c r="F13" s="16"/>
+      <c r="H13" s="8">
+        <v>0.36</v>
+      </c>
+      <c r="J13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" ht="9.5" customHeight="1" thickBot="1">
+      <c r="D14" s="2"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="12"/>
+    </row>
+    <row r="15" spans="2:10" ht="11.5" customHeight="1" thickBot="1">
+      <c r="D15" s="4"/>
+      <c r="F15" s="18"/>
+    </row>
+    <row r="16" spans="2:10" ht="18.5" thickBot="1">
+      <c r="D16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" s="14">
+        <v>0.1</v>
+      </c>
+      <c r="F16" s="19"/>
+      <c r="G16" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H16" s="14">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="J16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" ht="9" customHeight="1" thickBot="1">
+      <c r="D17" s="7"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="11"/>
+    </row>
+    <row r="18" spans="2:10" ht="18.5" thickBot="1">
+      <c r="D18" s="7"/>
+      <c r="G18" s="4"/>
+    </row>
+    <row r="19" spans="2:10" ht="18.5" thickBot="1">
+      <c r="D19" s="7"/>
+      <c r="G19" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H19" s="14">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="J19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" ht="9.5" customHeight="1" thickBot="1">
+      <c r="D20" s="7"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="11"/>
+    </row>
+    <row r="21" spans="2:10" ht="18.5" thickBot="1">
+      <c r="D21" s="7"/>
+      <c r="G21" s="4"/>
+    </row>
+    <row r="22" spans="2:10" ht="18.5" thickBot="1">
+      <c r="D22" s="7"/>
+      <c r="G22" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H22" s="14">
+        <v>0.01</v>
+      </c>
+      <c r="J22" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" ht="9.5" customHeight="1" thickBot="1">
+      <c r="H23" s="11"/>
+    </row>
+    <row r="25" spans="2:10">
+      <c r="B25" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25" s="8">
+        <f>SUMIF(J$4:J$22,B25,H$4:H$22)</f>
+        <v>0.23039999999999999</v>
+      </c>
+      <c r="F25" s="8"/>
+    </row>
+    <row r="26" spans="2:10">
+      <c r="B26" t="s">
+        <v>6</v>
+      </c>
+      <c r="E26" s="8">
+        <f>SUMIF(J$4:J$22,B26,H$4:H$22)</f>
+        <v>0.36</v>
+      </c>
+      <c r="F26" s="8"/>
+    </row>
+    <row r="27" spans="2:10" ht="18.5" thickBot="1">
+      <c r="B27" t="s">
+        <v>10</v>
+      </c>
+      <c r="E27" s="9">
+        <f>SUMIF(J$4:J$22,B27,H$4:H$22)</f>
+        <v>0.40960000000000002</v>
+      </c>
+      <c r="F27" s="15"/>
+    </row>
+    <row r="28" spans="2:10">
+      <c r="E28" s="8">
+        <f>SUM(E25:E27)</f>
+        <v>1</v>
+      </c>
+      <c r="F28" s="8"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26D7892D-F939-4E67-92C5-D425ACAE01A5}">
+  <dimension ref="A1:F8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18"/>
+  <cols>
+    <col min="2" max="2" width="18.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2">
+        <v>0.54</v>
+      </c>
+      <c r="E2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2">
+        <v>0.29160000000000003</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3">
+        <v>0.19439999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4">
+        <v>5.3999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6">
+        <v>0.1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6">
+        <v>5.3999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7">
+        <v>3.5999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8">
+        <v>0.01</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>